<commit_message>
added NACA0882(deleted by mistake), updated overview table. excluded trials over 20 to check what is going on
</commit_message>
<xml_diff>
--- a/TUS_BEHA_320trials_STUDY_1/HP-FouE-AI-010223-SESSIONS.xlsx
+++ b/TUS_BEHA_320trials_STUDY_1/HP-FouE-AI-010223-SESSIONS.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveplymouthac-my.sharepoint.com/personal/nomiki_koutsoumpari_plymouth_ac_uk/Documents/TARA/PhD/NEURO/PARTICIPANTS/TUS ONLY_STUDY_1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nkoutsoumpari\Documents\R\R\TUS_analysis\TUS_BEHA_320trials_STUDY_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="892" documentId="11_F25DC773A252ABDACC104846A15B52025BDE58F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41EC1B16-B00E-48BE-A7F7-F9EAD1C3DEEE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23259C19-A42E-414D-B1AA-5C898DE489DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-60" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
   <si>
     <t>sessions completed per participant</t>
   </si>
@@ -176,9 +176,6 @@
     <t>TBA-SEP-24</t>
   </si>
   <si>
-    <t>TBA-MAY-24</t>
-  </si>
-  <si>
     <t>name corrected for the sham it was originally saved as SSCH0384-CHANGED INTO PREPROC SCRIPT</t>
   </si>
   <si>
@@ -186,9 +183,6 @@
   </si>
   <si>
     <t>ai has 60-Nas at the end (last block) due to shorter parametrized file given (Elsa confirmed to keep it as it is)</t>
-  </si>
-  <si>
-    <t>D: 20/05/2024</t>
   </si>
   <si>
     <t>0 = not coming again</t>
@@ -389,7 +383,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -428,10 +422,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -758,7 +758,7 @@
   <dimension ref="A1:L42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -792,12 +792,12 @@
       <c r="A3"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="G3" s="19" t="s">
+      <c r="G3" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
       <c r="K3" s="11" t="s">
         <v>41</v>
       </c>
@@ -900,7 +900,7 @@
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8"/>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E8" s="2">
         <v>4</v>
@@ -925,7 +925,7 @@
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9"/>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E9" s="2">
         <v>5</v>
@@ -1012,7 +1012,7 @@
         <v>1</v>
       </c>
       <c r="K12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L12"/>
     </row>
@@ -1090,11 +1090,11 @@
       <c r="F16" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G16" s="15">
-        <v>1</v>
-      </c>
-      <c r="H16" s="15">
-        <v>1</v>
+      <c r="G16" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H16" s="15" t="s">
+        <v>44</v>
       </c>
       <c r="I16" s="15">
         <v>1</v>
@@ -1170,7 +1170,7 @@
       </c>
       <c r="L19"/>
     </row>
-    <row r="20" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20"/>
       <c r="E20" s="2">
         <v>16</v>
@@ -1192,7 +1192,7 @@
       </c>
       <c r="L20"/>
     </row>
-    <row r="21" spans="1:12" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21"/>
       <c r="E21" s="2">
         <v>17</v>
@@ -1200,10 +1200,10 @@
       <c r="F21" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G21" s="12">
-        <v>1</v>
-      </c>
-      <c r="H21" s="12">
+      <c r="G21" s="19">
+        <v>1</v>
+      </c>
+      <c r="H21" s="19">
         <v>1</v>
       </c>
       <c r="I21" s="15">
@@ -1217,7 +1217,7 @@
       </c>
       <c r="L21"/>
     </row>
-    <row r="22" spans="1:12" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22"/>
       <c r="E22" s="2">
         <v>18</v>
@@ -1269,11 +1269,11 @@
       <c r="F24" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G24" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="H24" s="15" t="s">
-        <v>44</v>
+      <c r="G24" s="19">
+        <v>1</v>
+      </c>
+      <c r="H24" s="19">
+        <v>1</v>
       </c>
       <c r="I24" s="16">
         <v>1</v>
@@ -1326,7 +1326,7 @@
         <v>1</v>
       </c>
       <c r="K26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L26"/>
     </row>
@@ -1351,7 +1351,7 @@
         <v>1</v>
       </c>
       <c r="K27" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="L27"/>
     </row>
@@ -1398,7 +1398,7 @@
         <v>1</v>
       </c>
       <c r="K29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L29"/>
     </row>
@@ -1423,7 +1423,7 @@
         <v>1</v>
       </c>
       <c r="K30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L30"/>
     </row>
@@ -1529,11 +1529,11 @@
       <c r="H35" s="15">
         <v>1</v>
       </c>
-      <c r="I35" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="J35" s="15" t="s">
-        <v>46</v>
+      <c r="I35" s="21">
+        <v>1</v>
+      </c>
+      <c r="J35" s="20">
+        <v>45439</v>
       </c>
       <c r="L35"/>
     </row>
@@ -1571,11 +1571,11 @@
       </c>
       <c r="I37" s="17">
         <f>SUM(I5:I36)</f>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J37" s="17">
         <f>SUM(J5:J36)</f>
-        <v>29</v>
+        <v>45468</v>
       </c>
       <c r="L37"/>
     </row>
@@ -1607,10 +1607,10 @@
     <mergeCell ref="G3:J3"/>
   </mergeCells>
   <conditionalFormatting sqref="B8:B1048576 B3">
-    <cfRule type="duplicateValues" dxfId="2" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:I5">
-    <cfRule type="colorScale" priority="17">
+    <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1621,8 +1621,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G6:I23 H24:I24 G25:I34">
-    <cfRule type="colorScale" priority="25">
+  <conditionalFormatting sqref="G6:I15 H16:I16 G17:I34">
+    <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1633,8 +1633,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G24">
-    <cfRule type="colorScale" priority="15">
+  <conditionalFormatting sqref="G16">
+    <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1646,6 +1646,30 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J5">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J6:J34">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -1657,8 +1681,11 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J5">
-    <cfRule type="colorScale" priority="11">
+  <conditionalFormatting sqref="F4:F34">
+    <cfRule type="duplicateValues" dxfId="1" priority="11"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J35:J36">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1669,22 +1696,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J6:J34">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF5A8AC6"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F4:F34">
-    <cfRule type="duplicateValues" dxfId="1" priority="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H35:H36 J35:J36">
+  <conditionalFormatting sqref="I35:I36">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -1696,23 +1708,11 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I35:I36">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF5A8AC6"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="F35:F36">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:D14">
-    <cfRule type="colorScale" priority="36">
+    <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1724,7 +1724,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D24">
-    <cfRule type="colorScale" priority="39">
+    <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1736,7 +1736,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:D13 C15:D23 C25:D34">
-    <cfRule type="colorScale" priority="40">
+    <cfRule type="colorScale" priority="41">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1748,6 +1748,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G35:G36">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H35:H36">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
some exclusions and new .csvs
</commit_message>
<xml_diff>
--- a/TUS_BEHA_320trials_STUDY_1/HP-FouE-AI-010223-SESSIONS.xlsx
+++ b/TUS_BEHA_320trials_STUDY_1/HP-FouE-AI-010223-SESSIONS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nkoutsoumpari\Documents\R\R\TUS_analysis\TUS_BEHA_320trials_STUDY_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23259C19-A42E-414D-B1AA-5C898DE489DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{079E0022-88CA-4D34-82C1-CBEC3D342561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-60" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
   <si>
     <t>sessions completed per participant</t>
   </si>
@@ -192,6 +192,9 @@
   </si>
   <si>
     <t>ai and dacc has 60-Nas at the end (last block) due to shorter parametrized file given (Elsa confirmed to keep it as it is)</t>
+  </si>
+  <si>
+    <t>TBA</t>
   </si>
 </sst>
 </file>
@@ -422,9 +425,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -432,6 +432,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -758,7 +761,7 @@
   <dimension ref="A1:L42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K37" sqref="K37"/>
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -792,12 +795,12 @@
       <c r="A3"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
       <c r="K3" s="11" t="s">
         <v>41</v>
       </c>
@@ -1200,10 +1203,10 @@
       <c r="F21" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G21" s="19">
-        <v>1</v>
-      </c>
-      <c r="H21" s="19">
+      <c r="G21" s="18">
+        <v>1</v>
+      </c>
+      <c r="H21" s="18">
         <v>1</v>
       </c>
       <c r="I21" s="15">
@@ -1269,10 +1272,10 @@
       <c r="F24" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G24" s="19">
-        <v>1</v>
-      </c>
-      <c r="H24" s="19">
+      <c r="G24" s="18">
+        <v>1</v>
+      </c>
+      <c r="H24" s="18">
         <v>1</v>
       </c>
       <c r="I24" s="16">
@@ -1529,11 +1532,11 @@
       <c r="H35" s="15">
         <v>1</v>
       </c>
-      <c r="I35" s="21">
-        <v>1</v>
-      </c>
-      <c r="J35" s="20">
-        <v>45439</v>
+      <c r="I35" s="20">
+        <v>1</v>
+      </c>
+      <c r="J35" s="19" t="s">
+        <v>52</v>
       </c>
       <c r="L35"/>
     </row>
@@ -1575,7 +1578,7 @@
       </c>
       <c r="J37" s="17">
         <f>SUM(J5:J36)</f>
-        <v>45468</v>
+        <v>29</v>
       </c>
       <c r="L37"/>
     </row>

</xml_diff>

<commit_message>
Add new logs and update analysis and preprocessing files
</commit_message>
<xml_diff>
--- a/TUS_BEHA_320trials_STUDY_1/HP-FouE-AI-010223-SESSIONS.xlsx
+++ b/TUS_BEHA_320trials_STUDY_1/HP-FouE-AI-010223-SESSIONS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nkoutsoumpari\Documents\R\R\TUS_analysis\TUS_BEHA_320trials_STUDY_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{742CFBAD-76F4-4FBD-A2AD-5A104BDF56E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{225FC714-E903-4C3A-AAF9-5F33279956C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-60" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
   <si>
     <t>sessions completed per participant</t>
   </si>
@@ -192,6 +192,12 @@
   </si>
   <si>
     <t>ai and dacc has 60-Nas at the end (last block) due to shorter parametrized file given (Elsa confirmed to keep it as it is)</t>
+  </si>
+  <si>
+    <t>QMDU0210</t>
+  </si>
+  <si>
+    <t>GNPR0120</t>
   </si>
 </sst>
 </file>
@@ -428,10 +434,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -755,10 +761,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L42"/>
+  <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -792,12 +798,12 @@
       <c r="A3"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
       <c r="K3" s="11" t="s">
         <v>41</v>
       </c>
@@ -1515,8 +1521,7 @@
       </c>
       <c r="L34"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35"/>
+    <row r="35" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E35" s="2">
         <v>31</v>
       </c>
@@ -1532,73 +1537,77 @@
       <c r="I35" s="19">
         <v>1</v>
       </c>
-      <c r="J35" s="21">
-        <v>1</v>
-      </c>
-      <c r="L35"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36"/>
-      <c r="E36" s="2">
+      <c r="J35" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E36" s="2"/>
+      <c r="F36" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G36" s="15"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E37" s="2"/>
+      <c r="F37" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E38" s="2">
         <v>32</v>
       </c>
-      <c r="F36" s="6" t="s">
+      <c r="F38" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="G36" s="15">
-        <v>1</v>
-      </c>
-      <c r="H36" s="15">
-        <v>1</v>
-      </c>
-      <c r="I36" s="15" t="s">
+      <c r="G38" s="15">
+        <v>1</v>
+      </c>
+      <c r="H38" s="15">
+        <v>1</v>
+      </c>
+      <c r="I38" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="J36" s="15" t="s">
+      <c r="J38" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="L36"/>
-    </row>
-    <row r="37" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37"/>
-      <c r="G37" s="17">
-        <f>SUM(G5:G36)</f>
+    </row>
+    <row r="39" spans="1:12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="G39" s="17">
+        <f>SUM(G5:G38)</f>
         <v>31</v>
       </c>
-      <c r="H37" s="17">
-        <f>SUM(H5:H36)</f>
+      <c r="H39" s="17">
+        <f>SUM(H5:H38)</f>
         <v>31</v>
       </c>
-      <c r="I37" s="17">
-        <f>SUM(I5:I36)</f>
+      <c r="I39" s="17">
+        <f>SUM(I5:I38)</f>
         <v>29</v>
       </c>
-      <c r="J37" s="17">
-        <f>SUM(J5:J36)</f>
-        <v>30</v>
-      </c>
-      <c r="L37"/>
-    </row>
-    <row r="38" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38"/>
-      <c r="L38"/>
-    </row>
-    <row r="39" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39"/>
-      <c r="L39"/>
-    </row>
-    <row r="40" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40"/>
-      <c r="L40"/>
-    </row>
-    <row r="41" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41"/>
-      <c r="L41"/>
-    </row>
-    <row r="42" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42"/>
-      <c r="L42"/>
-    </row>
+      <c r="J39" s="17">
+        <f>SUM(J5:J38)</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:12" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:12" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:12" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:12" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:B34">
     <sortCondition ref="B5:B34"/>
@@ -1621,7 +1630,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G6:I15 H16:I16 G17:I34">
+  <conditionalFormatting sqref="G6:I15 H16:I16 G17:I34 I36">
     <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
@@ -1684,7 +1693,7 @@
   <conditionalFormatting sqref="F4:F34">
     <cfRule type="duplicateValues" dxfId="1" priority="11"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J35:J36">
+  <conditionalFormatting sqref="J35:J38">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -1696,7 +1705,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I35:I36">
+  <conditionalFormatting sqref="I37:I38 I35">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -1708,7 +1717,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F35:F36">
+  <conditionalFormatting sqref="F35:F38">
     <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:D14">
@@ -1747,7 +1756,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G35:G36">
+  <conditionalFormatting sqref="G35:G38">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1759,7 +1768,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H35:H36">
+  <conditionalFormatting sqref="H35:H38">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>